<commit_message>
2.6, 4: 5 test cases added
todo: write the results of the test cases into the table
</commit_message>
<xml_diff>
--- a/tablazatok/teszteles.xlsx
+++ b/tablazatok/teszteles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bence\Documents\GitHub\oprendszerek_beadando\tablazatok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagytoth\Documents\repo\oprendszerek_beadando\tablazatok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FEFC89-D580-41D9-946D-6C160ED5B383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45E6769-DE5B-46E1-8DD6-A80B10E53DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-120" windowWidth="27900" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="-110" windowWidth="18020" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teszt terv" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="109">
   <si>
     <t>Elvárt eredmény</t>
   </si>
@@ -298,6 +298,66 @@
   </si>
   <si>
     <t>Teszt azonosítója</t>
+  </si>
+  <si>
+    <t>WEB_01</t>
+  </si>
+  <si>
+    <t>WEB_02</t>
+  </si>
+  <si>
+    <t>Az iskola weboldalán működik a navigációs sáv</t>
+  </si>
+  <si>
+    <t>Weboldalak megvalósítását teszteljük</t>
+  </si>
+  <si>
+    <t>Az iskola weboldalán elérhetőek, letölthetőek az érettségi tételek</t>
+  </si>
+  <si>
+    <t>Az iskola weboldalára működik a névfeloldás</t>
+  </si>
+  <si>
+    <t>NET_26</t>
+  </si>
+  <si>
+    <t>A router DNS-konfigurációját teszteljük</t>
+  </si>
+  <si>
+    <t>NET_27</t>
+  </si>
+  <si>
+    <t>Az Internal gépei ki tudnak menni az internetre, a névfeloldás interneten is működik</t>
+  </si>
+  <si>
+    <t>A kliensek Cloudflare DNS-szerverrel való kapcsolatát teszteljük</t>
+  </si>
+  <si>
+    <t>NET_28</t>
+  </si>
+  <si>
+    <t>Az Internalon kívüli alhálózatok is ki tudnak menni az internetre, a névfeloldás számukra is működik</t>
+  </si>
+  <si>
+    <t>Tetszőleges kliensgépen ping www.blg.lan parancsot futtattuk terminálban</t>
+  </si>
+  <si>
+    <t>Az iskola honlapján a navigációs sáv 
+gombjaira kattintgatunk, és figyeljük, hogy mindegyik gomb megfelelő helyre irányít-e.</t>
+  </si>
+  <si>
+    <t>Az "Érettségi" oldalon a kitűzött tematikák linkjeire kattintunk, és figyeljük, hogy a letöltés elkezdődik-e.</t>
+  </si>
+  <si>
+    <t>Winbox programba beírjuk a router ether1 interfészének címét (Mikrotikben /ip address print), és beírjuk az adminisztrátor jelszavát. A teszt sikeres akkor, ha a konfigurációs felületet látjuk.</t>
+  </si>
+  <si>
+    <t>gepterem1 és gepterem2 és gepterem3 alhálózatra kapcsolt kliensgépen 
+ping 8.8.8.8 és ping google.hu parancsokat futtattuk terminálban</t>
+  </si>
+  <si>
+    <t>Internal alhálózatra kapcsolt kliensgépen 
+ping 8.8.8.8 és ping google.hu parancsokat futtattuk terminálban</t>
   </si>
 </sst>
 </file>
@@ -305,7 +365,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -370,7 +430,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -384,9 +444,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -669,21 +738,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="A1:D26"/>
+      <selection activeCell="A27" sqref="A27:D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -697,7 +766,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -711,7 +780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -725,7 +794,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -739,7 +808,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -753,7 +822,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -767,7 +836,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -781,7 +850,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -795,7 +864,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -809,7 +878,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -823,7 +892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -837,7 +906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -851,7 +920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -865,7 +934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -879,7 +948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -893,7 +962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -907,7 +976,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -921,7 +990,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -935,7 +1004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -949,7 +1018,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -963,7 +1032,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -977,7 +1046,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -991,7 +1060,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
@@ -1005,7 +1074,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
@@ -1019,7 +1088,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
@@ -1033,7 +1102,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -1045,6 +1114,76 @@
       </c>
       <c r="D26" s="3" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1056,46 +1195,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B792DB35-53F5-4701-9F31-9F764EE1E7EE}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection sqref="A1:E26"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1105,14 +1244,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -1122,14 +1261,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -1139,14 +1278,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1156,14 +1295,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -1173,14 +1312,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1190,14 +1329,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1207,14 +1346,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1224,14 +1363,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1241,14 +1380,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1258,14 +1397,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -1275,14 +1414,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1292,14 +1431,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1309,14 +1448,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1326,14 +1465,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1343,14 +1482,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -1360,14 +1499,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1377,14 +1516,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -1394,14 +1533,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1411,14 +1550,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1428,14 +1567,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1445,14 +1584,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -1462,14 +1601,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1479,14 +1618,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1496,14 +1635,14 @@
         <v>45262</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -1511,6 +1650,76 @@
       </c>
       <c r="E26" s="7">
         <v>45262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="7">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="7">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="7">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="7">
+        <v>45265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>